<commit_message>
Improved in selection(now you can choose RWS or Ranked).Improved Crossover.now algorithm uses DSGA for diversity improvement!
</commit_message>
<xml_diff>
--- a/Amoozesh.xlsx
+++ b/Amoozesh.xlsx
@@ -1,40 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28908"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amirhosseinrahimi/Downloads/information/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,16 +80,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -116,12 +126,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -148,15 +158,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -183,7 +192,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -359,33 +367,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>100</v>
-      </c>
-      <c r="B1">
-        <v>105</v>
-      </c>
-      <c r="C1">
-        <v>110</v>
-      </c>
-      <c r="D1">
-        <v>115</v>
-      </c>
-      <c r="E1">
-        <v>120</v>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>